<commit_message>
tested the income statement document generator
</commit_message>
<xml_diff>
--- a/data/Expenses Payables (OUT).xlsx
+++ b/data/Expenses Payables (OUT).xlsx
@@ -405,7 +405,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Payment Date</v>
+        <v>Date</v>
       </c>
       <c r="B1" t="str">
         <v>Invoice/Receipt Number</v>
@@ -533,10 +533,10 @@
         <v>EUR</v>
       </c>
       <c r="E5" t="str">
-        <v>664</v>
+        <v>4000</v>
       </c>
       <c r="F5" t="str">
-        <v>Unpaid</v>
+        <v>Paid</v>
       </c>
       <c r="G5" t="str">
         <v>2023-02-23</v>

</xml_diff>